<commit_message>
add and update files
</commit_message>
<xml_diff>
--- a/lendingrisk/新建 Microsoft Excel 工作表.xlsx
+++ b/lendingrisk/新建 Microsoft Excel 工作表.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3881065B-4C77-438C-BA55-9FDF09C67FED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD622E12-EDED-4912-9528-9A936CAB77EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -649,6 +649,20 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -661,43 +675,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1764,7 +1764,7 @@
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="16" t="s">
         <v>84</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1773,7 +1773,7 @@
       <c r="C3" s="1">
         <v>0.15687483999999999</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="16" t="s">
         <v>130</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1788,7 +1788,7 @@
       <c r="K3" s="1">
         <v>8.6779473260664E-2</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="16" t="s">
         <v>138</v>
       </c>
       <c r="N3" s="1" t="s">
@@ -1799,14 +1799,14 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="10"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C4" s="1">
         <v>0.10904612</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="16"/>
       <c r="F4" s="1" t="s">
         <v>87</v>
       </c>
@@ -1819,7 +1819,7 @@
       <c r="K4" s="1">
         <v>8.3156358646470196E-2</v>
       </c>
-      <c r="M4" s="10"/>
+      <c r="M4" s="16"/>
       <c r="N4" s="1" t="s">
         <v>88</v>
       </c>
@@ -1828,14 +1828,14 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="10"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="1">
         <v>1.7676646000000001E-2</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="16"/>
       <c r="F5" s="1" t="s">
         <v>88</v>
       </c>
@@ -1848,7 +1848,7 @@
       <c r="K5" s="1">
         <v>7.7924457655247206E-2</v>
       </c>
-      <c r="M5" s="10"/>
+      <c r="M5" s="16"/>
       <c r="N5" s="1" t="s">
         <v>87</v>
       </c>
@@ -1857,14 +1857,14 @@
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="10"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C6" s="1">
         <v>1.5471423E-2</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="16"/>
       <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1877,7 +1877,7 @@
       <c r="K6" s="1">
         <v>5.8626868320961603E-2</v>
       </c>
-      <c r="M6" s="10"/>
+      <c r="M6" s="16"/>
       <c r="N6" s="1" t="s">
         <v>101</v>
       </c>
@@ -1886,14 +1886,14 @@
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="10"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C7" s="1">
         <v>1.4887176E-2</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="16"/>
       <c r="F7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1906,7 +1906,7 @@
       <c r="K7" s="1">
         <v>4.6898540701750799E-2</v>
       </c>
-      <c r="M7" s="10"/>
+      <c r="M7" s="16"/>
       <c r="N7" s="1" t="s">
         <v>129</v>
       </c>
@@ -1915,14 +1915,14 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="10"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C8" s="1">
         <v>1.3480304E-2</v>
       </c>
-      <c r="E8" s="10"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="1" t="s">
         <v>89</v>
       </c>
@@ -1935,7 +1935,7 @@
       <c r="K8" s="1">
         <v>4.5084838918122899E-2</v>
       </c>
-      <c r="M8" s="10"/>
+      <c r="M8" s="16"/>
       <c r="N8" s="1" t="s">
         <v>128</v>
       </c>
@@ -1944,14 +1944,14 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="10"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="1">
         <v>1.3272760999999999E-2</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="16"/>
       <c r="F9" s="1" t="s">
         <v>43</v>
       </c>
@@ -1964,7 +1964,7 @@
       <c r="K9" s="1">
         <v>4.2568888878130998E-2</v>
       </c>
-      <c r="M9" s="10"/>
+      <c r="M9" s="16"/>
       <c r="N9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1973,14 +1973,14 @@
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="10"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C10" s="1">
         <v>1.2245466E-2</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="1" t="s">
         <v>90</v>
       </c>
@@ -1993,7 +1993,7 @@
       <c r="K10" s="1">
         <v>4.0034278152206802E-2</v>
       </c>
-      <c r="M10" s="10"/>
+      <c r="M10" s="16"/>
       <c r="N10" s="1" t="s">
         <v>91</v>
       </c>
@@ -2080,7 +2080,7 @@
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="11">
+      <c r="A14" s="17">
         <v>0.73441130689071998</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2089,7 +2089,7 @@
       <c r="C14" s="1">
         <v>6.3687893999999998E-3</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="18">
         <v>0.73510656551536202</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -2104,7 +2104,7 @@
       <c r="K14" s="1">
         <v>2.6720790086233299E-2</v>
       </c>
-      <c r="M14" s="12">
+      <c r="M14" s="18">
         <v>0.72997009436355098</v>
       </c>
       <c r="N14" s="1" t="s">
@@ -2115,14 +2115,14 @@
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="11"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="1">
         <v>6.3161880000000004E-3</v>
       </c>
-      <c r="E15" s="12"/>
+      <c r="E15" s="18"/>
       <c r="F15" s="1" t="s">
         <v>96</v>
       </c>
@@ -2135,7 +2135,7 @@
       <c r="K15" s="1">
         <v>2.6108165300773999E-2</v>
       </c>
-      <c r="M15" s="12"/>
+      <c r="M15" s="18"/>
       <c r="N15" s="1" t="s">
         <v>104</v>
       </c>
@@ -2144,14 +2144,14 @@
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="11"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="1">
         <v>6.0761160000000003E-3</v>
       </c>
-      <c r="E16" s="12"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="1" t="s">
         <v>10</v>
       </c>
@@ -2164,7 +2164,7 @@
       <c r="K16" s="1">
         <v>2.24612101712004E-2</v>
       </c>
-      <c r="M16" s="12"/>
+      <c r="M16" s="18"/>
       <c r="N16" s="1" t="s">
         <v>94</v>
       </c>
@@ -2173,14 +2173,14 @@
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="11"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="1">
         <v>6.0167494000000002E-3</v>
       </c>
-      <c r="E17" s="12"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="1" t="s">
         <v>44</v>
       </c>
@@ -2193,7 +2193,7 @@
       <c r="K17" s="1">
         <v>2.0578158165285802E-2</v>
       </c>
-      <c r="M17" s="12"/>
+      <c r="M17" s="18"/>
       <c r="N17" s="1" t="s">
         <v>7</v>
       </c>
@@ -2202,14 +2202,14 @@
       </c>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="11"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C18" s="1">
         <v>5.856338E-3</v>
       </c>
-      <c r="E18" s="12"/>
+      <c r="E18" s="18"/>
       <c r="F18" s="1" t="s">
         <v>31</v>
       </c>
@@ -2222,7 +2222,7 @@
       <c r="K18" s="1">
         <v>1.8603863970834401E-2</v>
       </c>
-      <c r="M18" s="12"/>
+      <c r="M18" s="18"/>
       <c r="N18" s="1" t="s">
         <v>127</v>
       </c>
@@ -2231,14 +2231,14 @@
       </c>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="11"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C19" s="1">
         <v>5.7501499999999999E-3</v>
       </c>
-      <c r="E19" s="12"/>
+      <c r="E19" s="18"/>
       <c r="F19" s="1" t="s">
         <v>42</v>
       </c>
@@ -2251,7 +2251,7 @@
       <c r="K19" s="1">
         <v>1.6565634807779901E-2</v>
       </c>
-      <c r="M19" s="12"/>
+      <c r="M19" s="18"/>
       <c r="N19" s="1" t="s">
         <v>90</v>
       </c>
@@ -2260,14 +2260,14 @@
       </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="11"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="1">
         <v>5.6187412999999997E-3</v>
       </c>
-      <c r="E20" s="12"/>
+      <c r="E20" s="18"/>
       <c r="F20" s="1" t="s">
         <v>94</v>
       </c>
@@ -2280,7 +2280,7 @@
       <c r="K20" s="1">
         <v>1.5240059612740499E-2</v>
       </c>
-      <c r="M20" s="12"/>
+      <c r="M20" s="18"/>
       <c r="N20" s="1" t="s">
         <v>107</v>
       </c>
@@ -2307,7 +2307,7 @@
       <c r="K21" s="1">
         <v>1.45933149076039E-2</v>
       </c>
-      <c r="M21" s="9">
+      <c r="M21" s="15">
         <v>0.72777140027012199</v>
       </c>
       <c r="N21" s="1" t="s">
@@ -2336,7 +2336,7 @@
       <c r="K22" s="1">
         <v>1.2850105397304299E-2</v>
       </c>
-      <c r="M22" s="9"/>
+      <c r="M22" s="15"/>
       <c r="N22" s="1" t="s">
         <v>43</v>
       </c>
@@ -2363,7 +2363,7 @@
       <c r="K23" s="1">
         <v>1.14794267665998E-2</v>
       </c>
-      <c r="M23" s="9"/>
+      <c r="M23" s="15"/>
       <c r="N23" s="1" t="s">
         <v>92</v>
       </c>
@@ -2390,7 +2390,7 @@
       <c r="K24" s="1">
         <v>1.0891291274876201E-2</v>
       </c>
-      <c r="M24" s="9"/>
+      <c r="M24" s="15"/>
       <c r="N24" s="1" t="s">
         <v>11</v>
       </c>
@@ -2417,7 +2417,7 @@
       <c r="K25" s="1">
         <v>1.02821238073545E-2</v>
       </c>
-      <c r="M25" s="9"/>
+      <c r="M25" s="15"/>
       <c r="N25" s="1" t="s">
         <v>103</v>
       </c>
@@ -4227,117 +4227,108 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="16"/>
-    <col min="5" max="5" width="23.44140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="16"/>
+    <col min="1" max="1" width="15.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="11"/>
+    <col min="5" max="5" width="23.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="14" customFormat="1" ht="32.4">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:18" s="10" customFormat="1" ht="32.4">
+      <c r="A1" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-    </row>
-    <row r="2" spans="1:18" s="22" customFormat="1" ht="32.4">
-      <c r="A2" s="20"/>
-      <c r="B2" s="26" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+    </row>
+    <row r="2" spans="1:18" s="13" customFormat="1" ht="32.4">
+      <c r="A2" s="21"/>
+      <c r="B2" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="18" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-    </row>
-    <row r="3" spans="1:18" s="25" customFormat="1" ht="17.399999999999999">
-      <c r="A3" s="23"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+    </row>
+    <row r="3" spans="1:18" s="14" customFormat="1" ht="17.399999999999999">
+      <c r="A3" s="22"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="12">
         <v>0.69187878613340503</v>
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="9">
         <v>0.72997009436355098</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
     <mergeCell ref="B1:O1"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -4348,8 +4339,18 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>